<commit_message>
update tools closes #13
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t xml:space="preserve">Tweezers, Idealtek Anti-Magnetic No. 7 Very Fine, Curved Tips</t>
   </si>
@@ -79,16 +79,25 @@
     <t xml:space="preserve">Eyeglass, Black No. 3.5 = 2.8x (Bergeon 4422-3.5)</t>
   </si>
   <si>
+    <t xml:space="preserve">White Cotton Gloves (Lint Free) Ladies Size - , retail. (T83814S)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H&amp;S Walsh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screwdriver Ø1.60mm Bergeon 30080-H - HS1416 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dust Cover &amp; Tray Divided For Watch Movements – HM71</t>
+  </si>
+  <si>
     <t xml:space="preserve">Basket 25mm Mini Watch Part Cleaning Basket Economy - HB125 </t>
   </si>
   <si>
-    <t xml:space="preserve">H &amp; S Walsh</t>
-  </si>
-  <si>
     <t xml:space="preserve">Basket Ø21mm x 11mm Mini Watch Part Cleaning Basket Economy - HB120 </t>
   </si>
   <si>
-    <t xml:space="preserve">Latex ESD Finger Protection Thimble Cots Medium (Pack Of 144) Bergeon 7968-18 - HP7968-18 </t>
+    <t xml:space="preserve">Latex ESD Finger Protection Thimble Cots Medium (Pack Of 144) Bergeon 7968-18</t>
   </si>
   <si>
     <t xml:space="preserve">Eyeglass 3.3x Magnification Black Plastic Watchmakers Bergeon 4422-3 - HE4422-3 </t>
@@ -127,25 +136,22 @@
     <t xml:space="preserve">Barrel press</t>
   </si>
   <si>
-    <t xml:space="preserve">Syntalube (2ml)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can’t find the receipt for these so just a guess!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moebius 8300 (10ml)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renata essence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bergeon oiler (green)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bergeon oiler (red)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bergeon case cushion</t>
+    <t xml:space="preserve">Oil Synt-A-Lube Moebius 9010 (2ml) – HO9010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grease Natural Moebius 8300 20ml - HG8300 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hairspring Degreasing Degreaser 250ml Essence of Renata – HF6013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oiler (Large) Green Bergeon 30102-C – HO30102-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oiler (Small) Red Bergeon 30102-A - HO30102-A (HO30102-A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case Cushion Watch Black Gel Ø75mm Bergeon 5395-75-N – HC5395-75-N</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -233,7 +239,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,6 +262,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -275,10 +285,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -435,32 +445,34 @@
         <v>7.95</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2"/>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>1.66</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="2" t="n">
-        <v>5.95</v>
+      <c r="B22" s="1" t="n">
+        <v>3.23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,15 +480,16 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>7.95</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="C23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>11.45</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,7 +497,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,21 +505,23 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="n">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2" t="n">
         <v>11.45</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>22.99</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,40 +529,38 @@
         <v>29</v>
       </c>
       <c r="B29" s="2" t="n">
+        <v>11.45</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>22.99</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2" t="n">
         <v>3.9</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="2" t="n">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2" t="n">
         <f aca="false">40*0.8</f>
         <v>32</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="2" t="n">
-        <f aca="false">9*0.8</f>
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="n">
-        <f aca="false">19.99*0.8</f>
-        <v>15.992</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,18 +568,22 @@
         <v>34</v>
       </c>
       <c r="B34" s="2" t="n">
-        <f aca="false">4.95*0.8</f>
-        <v>3.96</v>
-      </c>
+        <f aca="false">9*0.8</f>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="B36" s="2" t="n">
+        <f aca="false">19.99*0.8</f>
+        <v>15.992</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -574,63 +591,83 @@
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="C38" s="5"/>
+      <c r="B37" s="2" t="n">
+        <f aca="false">4.95*0.8</f>
+        <v>3.96</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C39" s="5"/>
+        <v>19.38</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="4" t="n">
-        <v>2</v>
+        <v>12.9</v>
       </c>
       <c r="C40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="n">
+        <v>7.86</v>
+      </c>
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="C41" s="5"/>
+      <c r="B42" s="4" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="n">
-        <f aca="false">SUM(B1:B41)</f>
-        <v>434.752</v>
-      </c>
+      <c r="B43" s="6" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="C43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="n">
-        <f aca="false">B43*1.2</f>
-        <v>521.7024</v>
+      <c r="B44" s="4" t="n">
+        <v>26.78</v>
+      </c>
+      <c r="C44" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <f aca="false">SUM(B1:B44)</f>
+        <v>441.452</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <f aca="false">B46*1.2</f>
+        <v>529.7424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>